<commit_message>
Added new Tests and test files
</commit_message>
<xml_diff>
--- a/vendor-code-finder/src/test/resources/empty.xlsx
+++ b/vendor-code-finder/src/test/resources/empty.xlsx
@@ -16,6 +16,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -49,8 +53,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -331,14 +336,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="C5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="63" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>